<commit_message>
remove redundant lines to open created workbook and sheet
</commit_message>
<xml_diff>
--- a/ch13/exercises/merged.xlsx
+++ b/ch13/exercises/merged.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -360,8 +360,6 @@
         </is>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3"/>
     <row r="5">
       <c r="C5" t="inlineStr">
         <is>
@@ -370,10 +368,6 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D3"/>
-    <mergeCell ref="C5:D5"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>